<commit_message>
[update] New model with mean and variance
</commit_message>
<xml_diff>
--- a/documents/Z.xlsx
+++ b/documents/Z.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>p</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>SumVariance</t>
   </si>
 </sst>
 </file>
@@ -184,14 +187,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1930,17 +1926,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E38">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C38">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1951,35 +1947,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.81640625" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
+    <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6">
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2">
         <f>D2</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1991,10 +1988,10 @@
       </c>
       <c r="G3">
         <f>D2*(1-D2)</f>
-        <v>1.4775E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+        <v>2.4375000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2009,7 +2006,7 @@
         <v>2.3263478740408408</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
@@ -2018,7 +2015,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C7" s="12"/>
       <c r="F7" t="s">
         <v>4</v>
@@ -2027,10 +2024,13 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>0</v>
       </c>
@@ -2047,380 +2047,660 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <f t="shared" ref="H8:H10" si="0">F8+G8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>1</v>
       </c>
       <c r="C9" s="2">
         <f>SQRT($G$3)*$G$4+$G$2+C8</f>
-        <v>0.29777330181406425</v>
+        <v>0.38820094542408551</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D38" si="1">ROUNDUP(C9,0)</f>
+        <f t="shared" ref="D9:D38" si="0">ROUNDUP(C9,0)</f>
         <v>1</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
         <f>$G$2+F8</f>
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G9">
-        <f>SQRT($G$3)*$G$4+G8</f>
-        <v>0.28277330181406424</v>
+        <f>$G$3+G8</f>
+        <v>2.4375000000000001E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>0.29777330181406425</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+        <f>SQRT(G9)*$G$4</f>
+        <v>0.36320094542408549</v>
+      </c>
+      <c r="I9">
+        <f>F9+H9</f>
+        <v>0.38820094542408551</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>2</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:C38" si="2">SQRT($G$3)*$G$4+$G$2+C9</f>
-        <v>0.5955466036281285</v>
+        <f t="shared" ref="C10:C38" si="1">SQRT($G$3)*$G$4+$G$2+C9</f>
+        <v>0.77640189084817102</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
         <f>$G$2+F9</f>
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="G10">
-        <f>SQRT($G$3)*$G$4+G9</f>
-        <v>0.56554660362812847</v>
+        <f>$G$3+G9</f>
+        <v>4.8750000000000002E-2</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>0.5955466036281285</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+        <f>SQRT(G10)*$G$4</f>
+        <v>0.51364370288547201</v>
+      </c>
+      <c r="I10">
+        <f>F10+H10</f>
+        <v>0.56364370288547205</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>3</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.89331990544219275</v>
+        <f t="shared" si="1"/>
+        <v>1.1646028362722565</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
         <f>$G$2+F10</f>
-        <v>4.4999999999999998E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="G11">
-        <f>SQRT($G$3)*$G$4+G10</f>
-        <v>0.84831990544219271</v>
+        <f>$G$3+G10</f>
+        <v>7.3124999999999996E-2</v>
       </c>
       <c r="H11">
-        <f>F11+G11</f>
-        <v>0.89331990544219275</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+        <f>SQRT(G11)*$G$4</f>
+        <v>0.62908249083156687</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I28" si="2">F11+H11</f>
+        <v>0.70408249083156682</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>4</v>
       </c>
       <c r="C12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.552803781696342</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <f t="shared" ref="F12:F28" si="3">$G$2+F11</f>
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G28" si="4">$G$3+G11</f>
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H28" si="5">SQRT(G12)*$G$4</f>
+        <v>0.72640189084817097</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>1.191093207256257</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+        <v>0.82640189084817095</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>5</v>
       </c>
       <c r="C13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9410047271204276</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0.12187500000000001</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>0.8121420034604464</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="2"/>
-        <v>1.4888665090703213</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+        <v>0.9371420034604464</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>6</v>
       </c>
       <c r="C14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3292056725445129</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0.14625000000000002</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>0.88965699038545043</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="2"/>
-        <v>1.7866398108843855</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+        <v>1.0396569903854505</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>7</v>
       </c>
       <c r="C15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7174066179685985</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>0.17062500000000003</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>0.96093937753567304</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="2"/>
-        <v>2.0844131126984498</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+        <v>1.135939377535673</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>8</v>
       </c>
       <c r="C16" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1056075633926841</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0.19500000000000003</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>1.0272874057709442</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="2"/>
-        <v>2.382186414512514</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.2272874057709442</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>9</v>
       </c>
       <c r="C17" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4938085088167696</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>0.21937500000000004</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="5"/>
+        <v>1.0896028362722565</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="2"/>
-        <v>2.6799597163265783</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.3146028362722566</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
         <v>10</v>
       </c>
       <c r="C18" s="2">
+        <f t="shared" si="1"/>
+        <v>3.8820094542408552</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0.24375000000000005</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="5"/>
+        <v>1.1485422358666204</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="2"/>
-        <v>2.9777330181406425</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.3985422358666204</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>11</v>
       </c>
       <c r="C19" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2702103996649408</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>0.26812500000000006</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="5"/>
+        <v>1.2046012594740407</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="2"/>
-        <v>3.2755063199547068</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.4796012594740406</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <v>12</v>
       </c>
       <c r="C20" s="2">
+        <f t="shared" si="1"/>
+        <v>4.6584113450890259</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>0.29250000000000004</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="5"/>
+        <v>1.2581649816631342</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="2"/>
-        <v>3.573279621768771</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.5581649816631342</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <v>13</v>
       </c>
       <c r="C21" s="2">
+        <f t="shared" si="1"/>
+        <v>5.046612290513111</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
+        <f>$G$2+F20</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>0.31687500000000002</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>1.3095396320235384</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="2"/>
-        <v>3.8710529235828353</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.6345396320235384</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>14</v>
       </c>
       <c r="C22" s="2">
+        <f t="shared" si="1"/>
+        <v>5.4348132359371961</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>0.34125</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="5"/>
+        <v>1.3589735003293086</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="2"/>
-        <v>4.1688262253968995</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.7089735003293087</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <v>15</v>
       </c>
       <c r="C23" s="2">
+        <f t="shared" si="1"/>
+        <v>5.8230141813612812</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>0.36562499999999998</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="5"/>
+        <v>1.406671212954272</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="2"/>
-        <v>4.4665995272109633</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.781671212954272</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <v>16</v>
       </c>
       <c r="C24" s="2">
+        <f t="shared" si="1"/>
+        <v>6.2112151267853664</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>0.38999999999999996</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="5"/>
+        <v>1.4528037816963419</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="2"/>
-        <v>4.764372829025028</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.8528037816963421</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>17</v>
       </c>
       <c r="C25" s="2">
+        <f t="shared" si="1"/>
+        <v>6.5994160722094515</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
+        <f t="shared" si="3"/>
+        <v>0.4250000000000001</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>0.41437499999999994</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="5"/>
+        <v>1.4975158613076998</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="2"/>
-        <v>5.0621461308390927</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.9225158613076998</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <v>18</v>
       </c>
       <c r="C26" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9876170176335366</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.45000000000000012</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>0.43874999999999992</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="5"/>
+        <v>1.5409311086564157</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="2"/>
-        <v>5.3599194326531574</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1.9909311086564159</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>19</v>
       </c>
       <c r="C27" s="2">
+        <f t="shared" si="1"/>
+        <v>7.3758179630576217</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.47500000000000014</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>0.4631249999999999</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="5"/>
+        <v>1.5831562173020197</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="2"/>
-        <v>5.6576927344672221</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+        <v>2.0581562173020198</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="4">
         <v>20</v>
       </c>
       <c r="C28" s="2">
+        <f t="shared" si="1"/>
+        <v>7.7640189084817068</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>0.48749999999999988</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="5"/>
+        <v>1.6242840069208924</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="2"/>
-        <v>5.9554660362812868</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+        <v>2.1242840069208926</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
         <v>21</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="2"/>
-        <v>6.2532393380953515</v>
+        <f t="shared" si="1"/>
+        <v>8.1522198539057928</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="4">
         <v>22</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="2"/>
-        <v>6.5510126399094162</v>
+        <f t="shared" si="1"/>
+        <v>8.540420799329878</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
         <v>23</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="2"/>
-        <v>6.8487859417234809</v>
+        <f t="shared" si="1"/>
+        <v>8.9286217447539631</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="4">
         <v>24</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="2"/>
-        <v>7.1465592435375456</v>
+        <f t="shared" si="1"/>
+        <v>9.3168226901780482</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E32" s="2"/>
     </row>
@@ -2429,12 +2709,12 @@
         <v>25</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="2"/>
-        <v>7.4443325453516103</v>
+        <f t="shared" si="1"/>
+        <v>9.7050236356021333</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E33" s="2"/>
     </row>
@@ -2443,12 +2723,12 @@
         <v>26</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="2"/>
-        <v>7.742105847165675</v>
+        <f t="shared" si="1"/>
+        <v>10.093224581026218</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="E34" s="2"/>
     </row>
@@ -2457,12 +2737,12 @@
         <v>27</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="2"/>
-        <v>8.0398791489797397</v>
+        <f t="shared" si="1"/>
+        <v>10.481425526450304</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="E35" s="2"/>
     </row>
@@ -2471,12 +2751,12 @@
         <v>28</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="2"/>
-        <v>8.3376524507938043</v>
+        <f t="shared" si="1"/>
+        <v>10.869626471874389</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="E36" s="2"/>
     </row>
@@ -2485,12 +2765,12 @@
         <v>29</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" si="2"/>
-        <v>8.635425752607869</v>
+        <f t="shared" si="1"/>
+        <v>11.257827417298474</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="E37" s="2"/>
     </row>
@@ -2499,12 +2779,12 @@
         <v>30</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="2"/>
-        <v>8.9331990544219337</v>
+        <f t="shared" si="1"/>
+        <v>11.646028362722559</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="E38" s="2"/>
     </row>
@@ -2513,22 +2793,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E38">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C38">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:F11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="F9:F28">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixing the model for the correct formulation
</commit_message>
<xml_diff>
--- a/documents/Z.xlsx
+++ b/documents/Z.xlsx
@@ -187,21 +187,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -1926,17 +1912,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E38">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C38">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1949,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2134,7 +2120,7 @@
         <v>0.62908249083156687</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I28" si="2">F11+H11</f>
+        <f>F11+H11</f>
         <v>0.70408249083156682</v>
       </c>
     </row>
@@ -2152,19 +2138,19 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <f t="shared" ref="F12:F28" si="3">$G$2+F11</f>
+        <f t="shared" ref="F12:F28" si="2">$G$2+F11</f>
         <v>0.1</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:G28" si="4">$G$3+G11</f>
+        <f t="shared" ref="G12:G28" si="3">$G$3+G11</f>
         <v>9.7500000000000003E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:H28" si="5">SQRT(G12)*$G$4</f>
+        <f>SQRT(G12)*$G$4</f>
         <v>0.72640189084817097</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f>F12+H12</f>
         <v>0.82640189084817095</v>
       </c>
     </row>
@@ -2182,19 +2168,19 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="3"/>
-        <v>0.125</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="4"/>
         <v>0.12187500000000001</v>
       </c>
       <c r="H13">
-        <f t="shared" si="5"/>
+        <f>SQRT(G13)*$G$4</f>
         <v>0.8121420034604464</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f>F13+H13</f>
         <v>0.9371420034604464</v>
       </c>
     </row>
@@ -2212,19 +2198,19 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="3"/>
-        <v>0.15</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="4"/>
         <v>0.14625000000000002</v>
       </c>
       <c r="H14">
-        <f t="shared" si="5"/>
+        <f>SQRT(G14)*$G$4</f>
         <v>0.88965699038545043</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f>F14+H14</f>
         <v>1.0396569903854505</v>
       </c>
     </row>
@@ -2242,19 +2228,19 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="3"/>
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="4"/>
         <v>0.17062500000000003</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
+        <f>SQRT(G15)*$G$4</f>
         <v>0.96093937753567304</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f>F15+H15</f>
         <v>1.135939377535673</v>
       </c>
     </row>
@@ -2272,19 +2258,19 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="3"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="4"/>
         <v>0.19500000000000003</v>
       </c>
       <c r="H16">
-        <f t="shared" si="5"/>
+        <f>SQRT(G16)*$G$4</f>
         <v>1.0272874057709442</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>F16+H16</f>
         <v>1.2272874057709442</v>
       </c>
     </row>
@@ -2302,19 +2288,19 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="3"/>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="4"/>
         <v>0.21937500000000004</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
+        <f>SQRT(G17)*$G$4</f>
         <v>1.0896028362722565</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>F17+H17</f>
         <v>1.3146028362722566</v>
       </c>
     </row>
@@ -2332,19 +2318,19 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.24999999999999997</v>
       </c>
       <c r="G18">
-        <f t="shared" si="4"/>
+        <f>$G$3+G17</f>
         <v>0.24375000000000005</v>
       </c>
       <c r="H18">
-        <f t="shared" si="5"/>
+        <f>SQRT(G18)*$G$4</f>
         <v>1.1485422358666204</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f>F18+H18</f>
         <v>1.3985422358666204</v>
       </c>
     </row>
@@ -2362,19 +2348,19 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
+        <f t="shared" si="2"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="3"/>
-        <v>0.27499999999999997</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="4"/>
         <v>0.26812500000000006</v>
       </c>
       <c r="H19">
-        <f t="shared" si="5"/>
+        <f>SQRT(G19)*$G$4</f>
         <v>1.2046012594740407</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f>F19+H19</f>
         <v>1.4796012594740406</v>
       </c>
     </row>
@@ -2392,19 +2378,19 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
         <v>0.29250000000000004</v>
       </c>
       <c r="H20">
-        <f t="shared" si="5"/>
+        <f>SQRT(G20)*$G$4</f>
         <v>1.2581649816631342</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f>F20+H20</f>
         <v>1.5581649816631342</v>
       </c>
     </row>
@@ -2426,15 +2412,15 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.31687500000000002</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
+        <f>SQRT(G21)*$G$4</f>
         <v>1.3095396320235384</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f>F21+H21</f>
         <v>1.6345396320235384</v>
       </c>
     </row>
@@ -2452,19 +2438,19 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
+        <f t="shared" si="2"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="3"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="4"/>
         <v>0.34125</v>
       </c>
       <c r="H22">
-        <f t="shared" si="5"/>
+        <f>SQRT(G22)*$G$4</f>
         <v>1.3589735003293086</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f>F22+H22</f>
         <v>1.7089735003293087</v>
       </c>
     </row>
@@ -2482,19 +2468,19 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
+        <f t="shared" si="2"/>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="3"/>
-        <v>0.37500000000000006</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
         <v>0.36562499999999998</v>
       </c>
       <c r="H23">
-        <f t="shared" si="5"/>
+        <f>SQRT(G23)*$G$4</f>
         <v>1.406671212954272</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f>F23+H23</f>
         <v>1.781671212954272</v>
       </c>
     </row>
@@ -2512,19 +2498,19 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="3"/>
-        <v>0.40000000000000008</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
         <v>0.38999999999999996</v>
       </c>
       <c r="H24">
-        <f t="shared" si="5"/>
+        <f>SQRT(G24)*$G$4</f>
         <v>1.4528037816963419</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f>F24+H24</f>
         <v>1.8528037816963421</v>
       </c>
     </row>
@@ -2542,19 +2528,19 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2">
+        <f t="shared" si="2"/>
+        <v>0.4250000000000001</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="3"/>
-        <v>0.4250000000000001</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="4"/>
         <v>0.41437499999999994</v>
       </c>
       <c r="H25">
-        <f t="shared" si="5"/>
+        <f>SQRT(G25)*$G$4</f>
         <v>1.4975158613076998</v>
       </c>
       <c r="I25">
-        <f t="shared" si="2"/>
+        <f>F25+H25</f>
         <v>1.9225158613076998</v>
       </c>
     </row>
@@ -2572,19 +2558,19 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.45000000000000012</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="3"/>
-        <v>0.45000000000000012</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="4"/>
         <v>0.43874999999999992</v>
       </c>
       <c r="H26">
-        <f t="shared" si="5"/>
+        <f>SQRT(G26)*$G$4</f>
         <v>1.5409311086564157</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
+        <f>F26+H26</f>
         <v>1.9909311086564159</v>
       </c>
     </row>
@@ -2602,19 +2588,19 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2">
+        <f t="shared" si="2"/>
+        <v>0.47500000000000014</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="3"/>
-        <v>0.47500000000000014</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="4"/>
         <v>0.4631249999999999</v>
       </c>
       <c r="H27">
-        <f t="shared" si="5"/>
+        <f>SQRT(G27)*$G$4</f>
         <v>1.5831562173020197</v>
       </c>
       <c r="I27">
-        <f t="shared" si="2"/>
+        <f>F27+H27</f>
         <v>2.0581562173020198</v>
       </c>
     </row>
@@ -2632,19 +2618,19 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
+        <f t="shared" si="2"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="3"/>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="4"/>
         <v>0.48749999999999988</v>
       </c>
       <c r="H28">
-        <f t="shared" si="5"/>
+        <f>SQRT(G28)*$G$4</f>
         <v>1.6242840069208924</v>
       </c>
       <c r="I28">
-        <f t="shared" si="2"/>
+        <f>F28+H28</f>
         <v>2.1242840069208926</v>
       </c>
     </row>
@@ -2793,22 +2779,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E38">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C38">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F28">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>